<commit_message>
projeto aula 03 com env
</commit_message>
<xml_diff>
--- a/aula03/metadado/people_metadado_to_work.xlsx
+++ b/aula03/metadado/people_metadado_to_work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f054485a52af266/Impacta/DataOps_DE03/aula03/metadado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="8_{FD5A1D61-5EEC-4F52-A224-6C7B828AC811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6E15984-07F9-4000-BF2A-93FAFB468284}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="8_{FD5A1D61-5EEC-4F52-A224-6C7B828AC811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52F9AF43-4ECE-4A5C-AFEC-32E60A23FFAC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{56E82249-3F94-4ED0-8D74-558A49E5802A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{56E82249-3F94-4ED0-8D74-558A49E5802A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -600,22 +600,23 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C4" sqref="C4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -679,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -705,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -731,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -757,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -783,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -809,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -835,7 +836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -861,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -887,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -913,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -939,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -965,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -991,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>

</xml_diff>